<commit_message>
Updated auto retry asset xlsx
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 2\Traveloka_DataAutomation_Performer_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7258372-283E-4452-BDE8-8FAB1B8E7700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8AB210-7553-45CB-B2CF-A107DD16AB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2877,7 +2877,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>